<commit_message>
change status of implementation parents to green
</commit_message>
<xml_diff>
--- a/group04/org/Work plan.xlsx
+++ b/group04/org/Work plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morten Dreher\Desktop\DSM\DSM5\Projekt\Group 04\DSM-Group-04\group04\org\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Predator\Desktop\5.Semester\Projektarbeit ll\Gruppe4\DSM-Group-04\group04\org\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AF1CCC-BC29-4E08-89C4-0CBFDC8FBDA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390377E5-15EC-4D17-9A45-022A2991D74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,19 +187,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -480,28 +480,28 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
-    <col min="5" max="5" width="32.88671875" customWidth="1"/>
-    <col min="6" max="6" width="31.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
       <c r="C2" t="s">
         <v>24</v>
       </c>
@@ -511,21 +511,21 @@
       <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,14 +542,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -559,12 +559,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -589,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Set request burst task to green
</commit_message>
<xml_diff>
--- a/group04/org/Work plan.xlsx
+++ b/group04/org/Work plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morten Dreher\Desktop\DSM\DSM5\Projekt\Group 04\DSM-Group-04\group04\org\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C27C6-A1B1-4982-BE2D-6EBA5DA7133A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0A1E96-7D1D-427F-B398-83718B143522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,19 +228,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -528,7 +531,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,14 +546,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" t="s">
         <v>24</v>
       </c>
@@ -563,19 +566,19 @@
       <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -626,7 +629,7 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -667,10 +670,10 @@
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>